<commit_message>
more tweaks to the write-up and some of the code
</commit_message>
<xml_diff>
--- a/Work/results/processed_results.xlsx
+++ b/Work/results/processed_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="520" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -3303,16 +3303,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E875" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E875" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E875"/>
   <sortState ref="A2:E875">
     <sortCondition descending="1" ref="D1:D875"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Place" dataDxfId="6"/>
-    <tableColumn id="2" name="R^2_twitter" dataDxfId="5"/>
-    <tableColumn id="3" name="RMSE_Twitter" dataDxfId="4"/>
-    <tableColumn id="4" name="RMSE_L4F" dataDxfId="3"/>
+    <tableColumn id="1" name="Place" dataDxfId="4"/>
+    <tableColumn id="2" name="R^2_twitter" dataDxfId="3"/>
+    <tableColumn id="3" name="RMSE_Twitter" dataDxfId="2"/>
+    <tableColumn id="4" name="RMSE_L4F" dataDxfId="1"/>
     <tableColumn id="5" name="Best" dataDxfId="0">
       <calculatedColumnFormula>IF(Table8[[#This Row],[RMSE_Twitter]]&lt;Table8[[#This Row],[RMSE_L4F]], 1, 2)</calculatedColumnFormula>
     </tableColumn>
@@ -58703,7 +58703,7 @@
   <dimension ref="A1:E875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>